<commit_message>
Added build_CEFA_data_frame function to scrapeCEFA to build data frame given multiple IDs.  Created buildCEFAdata.r script to create a data frame (and save a file) with the CEFs in our universe. Fixed a couple of wrong IDs in CEFList.xlsx.
</commit_message>
<xml_diff>
--- a/Data/CEFList.xlsx
+++ b/Data/CEFList.xlsx
@@ -722,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2501,7 +2501,7 @@
         <v>1.83E-2</v>
       </c>
       <c r="I47">
-        <v>19918</v>
+        <v>199180</v>
       </c>
       <c r="J47" t="str">
         <f t="shared" si="5"/>
@@ -3678,7 +3678,7 @@
         <v>1.5300000000000001E-2</v>
       </c>
       <c r="I78">
-        <v>2145748</v>
+        <v>214748</v>
       </c>
       <c r="J78" t="str">
         <f t="shared" si="14"/>

</xml_diff>